<commit_message>
modificacion a Base demo
</commit_message>
<xml_diff>
--- a/Pagos.xlsx
+++ b/Pagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\areca\Desktop\IGLOBAL Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9350A4-EE03-4A12-ABB8-35598313A610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C2A951-97F2-4F28-AAB7-F7A681AC6AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Codigo</t>
   </si>
   <si>
-    <t>Cuota Prueba 1</t>
-  </si>
-  <si>
-    <t>Cuota Prueba 2</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -54,62 +48,65 @@
     <t>Cotizacion</t>
   </si>
   <si>
-    <t>rere</t>
-  </si>
-  <si>
-    <t>cdcdv</t>
-  </si>
-  <si>
-    <t>trwwthw</t>
-  </si>
-  <si>
-    <t>stthtsst</t>
-  </si>
-  <si>
-    <t>tshsthts</t>
-  </si>
-  <si>
-    <t>sthsthsdth</t>
-  </si>
-  <si>
-    <t>sthshstht</t>
-  </si>
-  <si>
-    <t>yynuiiuytred</t>
-  </si>
-  <si>
-    <t>nbfd</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>hbv</t>
-  </si>
-  <si>
-    <t>8132140K</t>
-  </si>
-  <si>
     <t>Transferencia</t>
   </si>
   <si>
     <t>MedioPago</t>
   </si>
   <si>
-    <t>152113900</t>
-  </si>
-  <si>
     <t>Cheque</t>
   </si>
   <si>
     <t>Contado</t>
+  </si>
+  <si>
+    <t>Documento 1</t>
+  </si>
+  <si>
+    <t>Documento 2</t>
+  </si>
+  <si>
+    <t>Documento 3</t>
+  </si>
+  <si>
+    <t>Documento 4</t>
+  </si>
+  <si>
+    <t>Documento 5</t>
+  </si>
+  <si>
+    <t>Documento 6</t>
+  </si>
+  <si>
+    <t>Documento 7</t>
+  </si>
+  <si>
+    <t>Documento 8</t>
+  </si>
+  <si>
+    <t>Documento 9</t>
+  </si>
+  <si>
+    <t>Documento 10</t>
+  </si>
+  <si>
+    <t>Documento 11</t>
+  </si>
+  <si>
+    <t>Documento 12</t>
+  </si>
+  <si>
+    <t>Documento 13</t>
+  </si>
+  <si>
+    <t>Documento 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +119,12 @@
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -161,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,12 +182,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -470,7 +467,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -487,22 +484,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -516,16 +513,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6">
-        <v>139968018</v>
+        <v>666666666</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -533,114 +530,114 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="6">
         <v>666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>450000</v>
+        <v>5000</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="7">
-        <v>73942772</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6">
+        <v>666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>100000</v>
+        <v>3000</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6">
+        <v>666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4000</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>123000</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="7">
-        <v>135399345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6">
+        <v>666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>7000</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="8">
-        <v>135800384</v>
+        <v>6</v>
+      </c>
+      <c r="G7" s="6">
+        <v>666666666</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -648,190 +645,190 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>456000</v>
+        <v>8000</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>10000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>19000</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>35000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>156000</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7">
-        <v>137282887</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>850000</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="8">
-        <v>138216446</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>87840</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>354000</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>152000</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>32111000</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="8">
-        <v>155490942</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>8654855</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="7">
-        <v>170676777</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>1000000</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="8">
-        <v>179654482</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>520000</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
       <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="6">
+        <v>666666666</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>65000</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="7">
-        <v>179699478</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>32000</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="8">
-        <v>113176725</v>
+        <v>6</v>
+      </c>
+      <c r="G15" s="6">
+        <v>666666666</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -851,6 +848,7 @@
       <c r="G20" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>